<commit_message>
Uploaded Files for KW19
</commit_message>
<xml_diff>
--- a/website/src/documents/Privat/Apollon_Aufwandserfassung.xlsx
+++ b/website/src/documents/Privat/Apollon_Aufwandserfassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhbwstg.sharepoint.com/sites/o365grpSWE-Projekt/Freigegebene Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3151" documentId="13_ncr:1_{CF72DE10-053D-F84A-BF2F-97DB33227B5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{18817244-8847-4EBA-A7D3-76E53BAFF7DB}"/>
+  <xr:revisionPtr revIDLastSave="3410" documentId="13_ncr:1_{CF72DE10-053D-F84A-BF2F-97DB33227B5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FC51AD-CCA3-4964-B152-1C6453361543}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="9" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="10" xr2:uid="{5DFA726E-B0C4-4500-AF96-5BC0FDCBA0B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Zeiterfassung KW 16" sheetId="8" r:id="rId8"/>
     <sheet name="Zeiterfassung KW 17" sheetId="9" r:id="rId9"/>
     <sheet name="Zeiterfassung KW 18" sheetId="10" r:id="rId10"/>
+    <sheet name="Zeiterfassung KW 19" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="251">
   <si>
     <r>
       <rPr>
@@ -761,6 +762,9 @@
     <t>Modellüberarbeitungen</t>
   </si>
   <si>
+    <t>DbContext überarbeitet und Entity Framework Core Anbindung</t>
+  </si>
+  <si>
     <t>Krankheitsbedingt ausgefallen</t>
   </si>
   <si>
@@ -794,7 +798,64 @@
     <t>Fehlerbehebung EF und daraus folgende Anpassungen an Tests und Model</t>
   </si>
   <si>
-    <t>DbContext überarbeitet und Entity Framework Core Anbindung</t>
+    <t>Betreuer Weeky</t>
+  </si>
+  <si>
+    <t>Ausbessern der Dungeon Konfiguration</t>
+  </si>
+  <si>
+    <t>Zsm. Mit Leon Jerke</t>
+  </si>
+  <si>
+    <t>Anbinden der Chat-Komponente</t>
+  </si>
+  <si>
+    <t>Anbinden der Master Ansicht</t>
+  </si>
+  <si>
+    <t>Frontend-Implementierung</t>
+  </si>
+  <si>
+    <t>Schreiben von Frontend Services</t>
+  </si>
+  <si>
+    <t>Schreiben von Controllern</t>
+  </si>
+  <si>
+    <t>Allgemeine Frontend Arbeit</t>
+  </si>
+  <si>
+    <t>Test und Player/MasterService</t>
+  </si>
+  <si>
+    <t>Bugfixes</t>
+  </si>
+  <si>
+    <t>GameController</t>
+  </si>
+  <si>
+    <t>ConfigController überarbeitet</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Wiki Erstellung</t>
+  </si>
+  <si>
+    <t>Produktvergleich zum Pflichtenheft</t>
+  </si>
+  <si>
+    <t>Test der Benutzbarkeit</t>
+  </si>
+  <si>
+    <t>PlayerService Implementierung</t>
+  </si>
+  <si>
+    <t>Sonstige Gameimplementierung</t>
+  </si>
+  <si>
+    <t>Bug Fixing</t>
   </si>
 </sst>
 </file>
@@ -804,7 +865,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,6 +956,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2544,7 +2612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3019,6 +3087,12 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="106" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3349,7 +3423,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3370,10 +3444,10 @@
       <c r="B2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="167"/>
+      <c r="D2" s="169"/>
     </row>
     <row r="3" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="76"/>
@@ -3393,12 +3467,12 @@
         <v>3</v>
       </c>
       <c r="C4" s="143">
-        <f>'Zeiterfassung KW 10'!J18+'Zeiterfassung KW 11'!J18+'Zeiterfassung KW 12'!J18+'Zeiterfassung KW 13'!J18+'Zeiterfassung KW 14'!J18+'Zeiterfassung KW 15'!J18+'Zeiterfassung KW 16'!J18+'Zeiterfassung KW 17'!J18+'Zeiterfassung KW 18'!J18</f>
-        <v>830.75</v>
+        <f>'Zeiterfassung KW 10'!J18+'Zeiterfassung KW 11'!J18+'Zeiterfassung KW 12'!J18+'Zeiterfassung KW 13'!J18+'Zeiterfassung KW 14'!J18+'Zeiterfassung KW 15'!J18+'Zeiterfassung KW 16'!J18+'Zeiterfassung KW 17'!J18+'Zeiterfassung KW 18'!J18+'Zeiterfassung KW 19'!J18</f>
+        <v>1001.25</v>
       </c>
       <c r="D4" s="152">
         <f>C4/8</f>
-        <v>103.84375</v>
+        <v>125.15625</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3415,12 +3489,12 @@
         <v>3</v>
       </c>
       <c r="C6" s="143">
-        <f>'Zeiterfassung KW 10'!G12+'Zeiterfassung KW 11'!G14+'Zeiterfassung KW 12'!G11+'Zeiterfassung KW 13'!G10+'Zeiterfassung KW 14'!G11+'Zeiterfassung KW 15'!G10+'Zeiterfassung KW 16'!G9+'Zeiterfassung KW 17'!G10+'Zeiterfassung KW 18'!G8</f>
-        <v>158.25</v>
+        <f>'Zeiterfassung KW 10'!G12+'Zeiterfassung KW 11'!G14+'Zeiterfassung KW 12'!G11+'Zeiterfassung KW 13'!G10+'Zeiterfassung KW 14'!G11+'Zeiterfassung KW 15'!G10+'Zeiterfassung KW 16'!G9+'Zeiterfassung KW 17'!G10+'Zeiterfassung KW 18'!G8+'Zeiterfassung KW 19'!G9</f>
+        <v>192</v>
       </c>
       <c r="D6" s="152">
         <f>C6/8</f>
-        <v>19.78125</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3438,12 +3512,12 @@
         <v>3</v>
       </c>
       <c r="C8" s="145">
-        <f>'Zeiterfassung KW 10'!G20+'Zeiterfassung KW 11'!G30+'Zeiterfassung KW 12'!G23+'Zeiterfassung KW 13'!G18+'Zeiterfassung KW 14'!G20+'Zeiterfassung KW 15'!G19+'Zeiterfassung KW 16'!G18+'Zeiterfassung KW 17'!G17+'Zeiterfassung KW 18'!G15</f>
-        <v>176.25</v>
+        <f>'Zeiterfassung KW 10'!G20+'Zeiterfassung KW 11'!G30+'Zeiterfassung KW 12'!G23+'Zeiterfassung KW 13'!G18+'Zeiterfassung KW 14'!G20+'Zeiterfassung KW 15'!G19+'Zeiterfassung KW 16'!G18+'Zeiterfassung KW 17'!G17+'Zeiterfassung KW 18'!G15+'Zeiterfassung KW 19'!G18</f>
+        <v>215</v>
       </c>
       <c r="D8" s="152">
         <f>C8/8</f>
-        <v>22.03125</v>
+        <v>26.875</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3460,12 +3534,12 @@
         <v>3</v>
       </c>
       <c r="C10" s="145">
-        <f>'Zeiterfassung KW 10'!G28+'Zeiterfassung KW 11'!G41+'Zeiterfassung KW 12'!G30+'Zeiterfassung KW 13'!G25+'Zeiterfassung KW 14'!G28+'Zeiterfassung KW 15'!G25+'Zeiterfassung KW 16'!G24+'Zeiterfassung KW 17'!G23+'Zeiterfassung KW 18'!G20</f>
-        <v>141.75</v>
+        <f>'Zeiterfassung KW 10'!G28+'Zeiterfassung KW 11'!G41+'Zeiterfassung KW 12'!G30+'Zeiterfassung KW 13'!G25+'Zeiterfassung KW 14'!G28+'Zeiterfassung KW 15'!G25+'Zeiterfassung KW 16'!G24+'Zeiterfassung KW 17'!G23+'Zeiterfassung KW 18'!G20+'Zeiterfassung KW 19'!G22</f>
+        <v>177.5</v>
       </c>
       <c r="D10" s="152">
         <f>C10/8</f>
-        <v>17.71875</v>
+        <v>22.1875</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3482,12 +3556,12 @@
         <v>3</v>
       </c>
       <c r="C12" s="145">
-        <f>'Zeiterfassung KW 10'!G35+'Zeiterfassung KW 11'!G51+'Zeiterfassung KW 12'!G39+'Zeiterfassung KW 13'!G33+'Zeiterfassung KW 14'!G37+'Zeiterfassung KW 15'!G35+'Zeiterfassung KW 16'!G32+'Zeiterfassung KW 17'!G29+'Zeiterfassung KW 18'!G23</f>
-        <v>83.25</v>
+        <f>'Zeiterfassung KW 10'!G35+'Zeiterfassung KW 11'!G51+'Zeiterfassung KW 12'!G39+'Zeiterfassung KW 13'!G33+'Zeiterfassung KW 14'!G37+'Zeiterfassung KW 15'!G35+'Zeiterfassung KW 16'!G32+'Zeiterfassung KW 17'!G29+'Zeiterfassung KW 18'!G23+'Zeiterfassung KW 19'!G30</f>
+        <v>102</v>
       </c>
       <c r="D12" s="152">
         <f>C12/8</f>
-        <v>10.40625</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3504,12 +3578,12 @@
         <v>3</v>
       </c>
       <c r="C14" s="145">
-        <f>'Zeiterfassung KW 10'!G42+'Zeiterfassung KW 11'!G63+'Zeiterfassung KW 12'!G48+'Zeiterfassung KW 13'!G40+'Zeiterfassung KW 14'!G46+'Zeiterfassung KW 15'!G44+'Zeiterfassung KW 16'!G38+'Zeiterfassung KW 17'!G38+'Zeiterfassung KW 18'!G19</f>
-        <v>103.75</v>
+        <f>'Zeiterfassung KW 10'!G42+'Zeiterfassung KW 11'!G63+'Zeiterfassung KW 12'!G48+'Zeiterfassung KW 13'!G40+'Zeiterfassung KW 14'!G46+'Zeiterfassung KW 15'!G44+'Zeiterfassung KW 16'!G38+'Zeiterfassung KW 17'!G38+'Zeiterfassung KW 18'!G19+'Zeiterfassung KW 19'!G37</f>
+        <v>125.5</v>
       </c>
       <c r="D14" s="152">
         <f>C14/8</f>
-        <v>12.96875</v>
+        <v>15.6875</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3526,12 +3600,12 @@
         <v>3</v>
       </c>
       <c r="C16" s="146">
-        <f>'Zeiterfassung KW 10'!G54+'Zeiterfassung KW 11'!G75+'Zeiterfassung KW 12'!G60+'Zeiterfassung KW 13'!G50+'Zeiterfassung KW 14'!G57+'Zeiterfassung KW 15'!G55+'Zeiterfassung KW 16'!G46+'Zeiterfassung KW 17'!G51+'Zeiterfassung KW 18'!G40</f>
-        <v>161.5</v>
+        <f>'Zeiterfassung KW 10'!G54+'Zeiterfassung KW 11'!G75+'Zeiterfassung KW 12'!G60+'Zeiterfassung KW 13'!G50+'Zeiterfassung KW 14'!G57+'Zeiterfassung KW 15'!G55+'Zeiterfassung KW 16'!G46+'Zeiterfassung KW 17'!G51+'Zeiterfassung KW 18'!G40+'Zeiterfassung KW 19'!G44</f>
+        <v>183.25</v>
       </c>
       <c r="D16" s="153">
         <f>C16/8</f>
-        <v>20.1875</v>
+        <v>22.90625</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3551,8 +3625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7845F4C-3F76-4CB2-9982-0E19EC39A5BE}">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3641,7 +3715,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="65">
-        <v>44312</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3670,7 +3744,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="66">
-        <v>44318</v>
+        <v>44325</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3727,7 +3801,7 @@
     <row r="8" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="107" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>22</v>
@@ -4115,7 +4189,7 @@
     <row r="23" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="165" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C23" s="36"/>
       <c r="D23" s="36"/>
@@ -4187,7 +4261,7 @@
     <row r="27" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="98" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>28</v>
@@ -4210,7 +4284,7 @@
     <row r="28" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="98" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C28" s="36" t="s">
         <v>22</v>
@@ -4233,7 +4307,7 @@
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="98" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C29" s="35" t="s">
         <v>22</v>
@@ -4256,7 +4330,7 @@
     <row r="30" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="98" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C30" s="35" t="s">
         <v>22</v>
@@ -4336,7 +4410,7 @@
     <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="98" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>28</v>
@@ -4359,7 +4433,7 @@
     <row r="35" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="98" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>22</v>
@@ -4382,7 +4456,7 @@
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="107" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>22</v>
@@ -4405,7 +4479,7 @@
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="107" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C37" s="36" t="s">
         <v>22</v>
@@ -4431,7 +4505,7 @@
     <row r="38" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="98" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C38" s="36" t="s">
         <v>22</v>
@@ -4454,7 +4528,7 @@
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="98" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C39" s="36" t="s">
         <v>22</v>
@@ -4477,7 +4551,7 @@
     <row r="40" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="108" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C40" s="111" t="s">
         <v>38</v>
@@ -4614,6 +4688,1118 @@
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB18F1A6-A401-4F95-ACF9-4D2A8A43B6C2}">
+  <dimension ref="A1:K68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="3"/>
+    <col min="9" max="9" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="53"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+    </row>
+    <row r="2" spans="1:11" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="166"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="47"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="65">
+        <v>44326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="99">
+        <f>E5</f>
+        <v>0.75</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="66">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="98" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="35">
+        <v>15</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="99">
+        <f>G5+E6</f>
+        <v>15.75</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="98" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="35">
+        <v>5</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="99">
+        <f>G6+E7</f>
+        <v>20.75</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="50"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="98" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="35">
+        <v>3</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="99">
+        <f>G7+E8</f>
+        <v>23.75</v>
+      </c>
+      <c r="H8" s="44"/>
+      <c r="I8" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="51"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="107" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="35">
+        <v>10</v>
+      </c>
+      <c r="F9" s="36"/>
+      <c r="G9" s="99">
+        <f>G8+E9</f>
+        <v>33.75</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="47"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="44"/>
+      <c r="I11" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F12" s="36"/>
+      <c r="G12" s="99">
+        <f>E12</f>
+        <v>0.75</v>
+      </c>
+      <c r="H12" s="44"/>
+      <c r="I12" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="98" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="35">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="G13" s="99">
+        <f>G12+E13</f>
+        <v>4.75</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="35">
+        <v>3</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="99">
+        <f t="shared" ref="G14:G18" si="0">G13+E14</f>
+        <v>7.75</v>
+      </c>
+      <c r="H14" s="44"/>
+      <c r="I14" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="35">
+        <v>10</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="99">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="98" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="35">
+        <v>3</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="99">
+        <f t="shared" si="0"/>
+        <v>20.75</v>
+      </c>
+      <c r="H16" s="44"/>
+      <c r="I16" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="68"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="98" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="35">
+        <v>1</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="99">
+        <f t="shared" si="0"/>
+        <v>21.75</v>
+      </c>
+      <c r="H17" s="44"/>
+      <c r="I17" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="98" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="35">
+        <v>17</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="99">
+        <f t="shared" si="0"/>
+        <v>38.75</v>
+      </c>
+      <c r="H18" s="44"/>
+      <c r="I18" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="83">
+        <f>SUM(G9,G18,G22,G37,G30,G44)</f>
+        <v>170.5</v>
+      </c>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="73">
+        <f>J18/5</f>
+        <v>34.1</v>
+      </c>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="44"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="99">
+        <f>E21</f>
+        <v>0.75</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+    </row>
+    <row r="22" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="98" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="35">
+        <v>35</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="99">
+        <f>G21+E22</f>
+        <v>35.75</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="99">
+        <f>E25</f>
+        <v>0.75</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="98" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="35">
+        <v>2</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="99">
+        <f>G25+E26</f>
+        <v>2.75</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="98" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="35">
+        <v>2</v>
+      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="99">
+        <f>G26+E27</f>
+        <v>4.75</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="98" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="35">
+        <v>5</v>
+      </c>
+      <c r="F28" s="36"/>
+      <c r="G28" s="99">
+        <f>G27+E28</f>
+        <v>9.75</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="98" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="35">
+        <v>5</v>
+      </c>
+      <c r="F29" s="36"/>
+      <c r="G29" s="99">
+        <f>G28+E29</f>
+        <v>14.75</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="167" t="s">
+        <v>247</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="35">
+        <v>4</v>
+      </c>
+      <c r="F30" s="36"/>
+      <c r="G30" s="99">
+        <f>G29+E30</f>
+        <v>18.75</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F33" s="36"/>
+      <c r="G33" s="99">
+        <f>E33</f>
+        <v>0.75</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="98" t="s">
+        <v>244</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="35">
+        <v>3</v>
+      </c>
+      <c r="F34" s="36"/>
+      <c r="G34" s="99">
+        <f>G33+E34</f>
+        <v>3.75</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="98" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="35">
+        <v>8</v>
+      </c>
+      <c r="F35" s="36"/>
+      <c r="G35" s="99">
+        <f t="shared" ref="G35:G37" si="1">G34+E35</f>
+        <v>11.75</v>
+      </c>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="98" t="s">
+        <v>246</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="35">
+        <v>5</v>
+      </c>
+      <c r="F36" s="36"/>
+      <c r="G36" s="99">
+        <f t="shared" si="1"/>
+        <v>16.75</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="98" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="35">
+        <v>5</v>
+      </c>
+      <c r="F37" s="36"/>
+      <c r="G37" s="99">
+        <f t="shared" si="1"/>
+        <v>21.75</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" s="99">
+        <f>E40</f>
+        <v>0.75</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="98" t="s">
+        <v>240</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="35">
+        <v>6</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="99">
+        <f>G40+E41</f>
+        <v>6.75</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="J41" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="98" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="35">
+        <v>6</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" s="99">
+        <f t="shared" ref="G42:G44" si="2">G41+E42</f>
+        <v>12.75</v>
+      </c>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="107" t="s">
+        <v>242</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="35">
+        <v>5</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="99">
+        <f t="shared" si="2"/>
+        <v>17.75</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="107" t="s">
+        <v>243</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="35">
+        <v>4</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="99">
+        <f t="shared" si="2"/>
+        <v>21.75</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="86"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="86"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="86"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="86"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="86"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="86"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="86"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="86"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="86"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="86"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="86"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="86"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="86"/>
+      <c r="H58" s="87"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="86"/>
+      <c r="H59" s="87"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="86"/>
+      <c r="H60" s="87"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="86"/>
+      <c r="H61" s="87"/>
+    </row>
+    <row r="62" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="86"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="86"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="86"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="86"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="86"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="86"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15984,14 +17170,14 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50F9D30A-50A2-408B-B3F0-EDB4CF8C0B75}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="9261f3b7-eb37-44bc-ab49-41e0f5c5a530"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>